<commit_message>
Insert calibration labels from rutger
</commit_message>
<xml_diff>
--- a/Scripts/FT_Screening_Bruno.xlsx
+++ b/Scripts/FT_Screening_Bruno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\Documents\Work related\Debugging\script_debugging\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAA34DE-58BD-468C-9892-4116B9D9844D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CC5B1A-FCC2-430D-9CBD-A617803122D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6236,12 +6236,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -6275,12 +6281,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6588,8 +6596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AN25" sqref="AN25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6755,171 +6763,171 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AO2">
-        <v>1</v>
-      </c>
-      <c r="AP2" t="s">
+      <c r="AB2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="3" t="s">
         <v>2048</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-      <c r="AP3" t="s">
+      <c r="AB3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AO3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="3" t="s">
         <v>2048</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:51" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AB4">
-        <v>1</v>
-      </c>
-      <c r="AC4">
-        <v>1</v>
-      </c>
-      <c r="AD4">
-        <v>1</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AO4">
-        <v>1</v>
-      </c>
-      <c r="AP4" t="s">
+      <c r="AB4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>2048</v>
       </c>
     </row>
@@ -12981,104 +12989,104 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="3" t="s">
         <v>839</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="3">
         <v>2014</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="3" t="s">
         <v>1045</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J67" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K67" s="3" t="s">
         <v>1235</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="L67" s="4" t="s">
         <v>1374</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M67" s="3" t="s">
         <v>1476</v>
       </c>
-      <c r="N67" t="s">
+      <c r="N67" s="3" t="s">
         <v>1533</v>
       </c>
-      <c r="O67" t="s">
+      <c r="O67" s="3" t="s">
         <v>1657</v>
       </c>
-      <c r="P67" t="s">
+      <c r="P67" s="3" t="s">
         <v>1749</v>
       </c>
-      <c r="Q67" t="s">
+      <c r="Q67" s="3" t="s">
         <v>1812</v>
       </c>
-      <c r="R67" t="s">
+      <c r="R67" s="3" t="s">
         <v>1850</v>
       </c>
-      <c r="S67" t="s">
+      <c r="S67" s="3" t="s">
         <v>1944</v>
       </c>
-      <c r="T67" t="s">
+      <c r="T67" s="3" t="s">
         <v>2000</v>
       </c>
-      <c r="AB67">
-        <v>1</v>
-      </c>
-      <c r="AC67">
-        <v>1</v>
-      </c>
-      <c r="AD67">
-        <v>1</v>
-      </c>
-      <c r="AE67">
-        <v>0</v>
-      </c>
-      <c r="AF67">
-        <v>0</v>
-      </c>
-      <c r="AG67">
-        <v>0</v>
-      </c>
-      <c r="AH67">
-        <v>0</v>
-      </c>
-      <c r="AI67" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ67" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AK67" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AL67" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM67" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AO67">
-        <v>1</v>
-      </c>
-      <c r="AP67" t="s">
+      <c r="AB67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI67" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ67" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AK67" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AL67" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM67" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AO67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP67" s="3" t="s">
         <v>2057</v>
       </c>
     </row>
@@ -15235,107 +15243,107 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="90" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="3">
         <v>2014</v>
       </c>
-      <c r="H90" t="s">
+      <c r="H90" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J90" s="3" t="s">
         <v>1142</v>
       </c>
-      <c r="K90" t="s">
+      <c r="K90" s="3" t="s">
         <v>1278</v>
       </c>
-      <c r="L90" s="2" t="s">
+      <c r="L90" s="4" t="s">
         <v>1397</v>
       </c>
-      <c r="M90" t="s">
+      <c r="M90" s="3" t="s">
         <v>1476</v>
       </c>
-      <c r="N90" t="s">
+      <c r="N90" s="3" t="s">
         <v>1553</v>
       </c>
-      <c r="O90" t="s">
+      <c r="O90" s="3" t="s">
         <v>1677</v>
       </c>
-      <c r="P90" t="s">
+      <c r="P90" s="3" t="s">
         <v>1764</v>
       </c>
-      <c r="Q90" t="s">
+      <c r="Q90" s="3" t="s">
         <v>1812</v>
       </c>
-      <c r="R90" t="s">
+      <c r="R90" s="3" t="s">
         <v>1859</v>
       </c>
-      <c r="S90" t="s">
+      <c r="S90" s="3" t="s">
         <v>1954</v>
       </c>
-      <c r="T90" t="s">
+      <c r="T90" s="3" t="s">
         <v>2018</v>
       </c>
-      <c r="AB90">
-        <v>1</v>
-      </c>
-      <c r="AC90">
-        <v>1</v>
-      </c>
-      <c r="AD90">
-        <v>1</v>
-      </c>
-      <c r="AE90">
-        <v>0</v>
-      </c>
-      <c r="AF90">
-        <v>0</v>
-      </c>
-      <c r="AG90">
-        <v>0</v>
-      </c>
-      <c r="AH90">
-        <v>0</v>
-      </c>
-      <c r="AI90" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ90" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AK90" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AL90" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM90" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AO90">
-        <v>1</v>
-      </c>
-      <c r="AP90" t="s">
+      <c r="AB90" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC90" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD90" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE90" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF90" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG90" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI90" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ90" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AK90" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AL90" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM90" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AO90" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP90" s="3" t="s">
         <v>2057</v>
       </c>
     </row>
@@ -22112,107 +22120,107 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="161" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+    <row r="161" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="F161" t="s">
+      <c r="F161" s="3" t="s">
         <v>933</v>
       </c>
-      <c r="G161">
+      <c r="G161" s="3">
         <v>2014</v>
       </c>
-      <c r="H161" t="s">
+      <c r="H161" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I161" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="J161" t="s">
+      <c r="J161" s="3" t="s">
         <v>1213</v>
       </c>
-      <c r="K161" t="s">
+      <c r="K161" s="3" t="s">
         <v>1278</v>
       </c>
-      <c r="L161" s="2" t="s">
+      <c r="L161" s="4" t="s">
         <v>1467</v>
       </c>
-      <c r="M161" t="s">
+      <c r="M161" s="3" t="s">
         <v>1476</v>
       </c>
-      <c r="N161" t="s">
+      <c r="N161" s="3" t="s">
         <v>1614</v>
       </c>
-      <c r="O161" t="s">
+      <c r="O161" s="3" t="s">
         <v>1677</v>
       </c>
-      <c r="P161" t="s">
+      <c r="P161" s="3" t="s">
         <v>1808</v>
       </c>
-      <c r="Q161" t="s">
+      <c r="Q161" s="3" t="s">
         <v>1812</v>
       </c>
-      <c r="R161" t="s">
+      <c r="R161" s="3" t="s">
         <v>1899</v>
       </c>
-      <c r="S161" t="s">
+      <c r="S161" s="3" t="s">
         <v>1990</v>
       </c>
-      <c r="T161" t="s">
+      <c r="T161" s="3" t="s">
         <v>2018</v>
       </c>
-      <c r="AB161">
-        <v>1</v>
-      </c>
-      <c r="AC161">
-        <v>1</v>
-      </c>
-      <c r="AD161">
-        <v>1</v>
-      </c>
-      <c r="AE161">
-        <v>0</v>
-      </c>
-      <c r="AF161">
-        <v>0</v>
-      </c>
-      <c r="AG161">
-        <v>0</v>
-      </c>
-      <c r="AH161">
-        <v>0</v>
-      </c>
-      <c r="AI161" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AJ161" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AK161" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AL161" t="s">
-        <v>2041</v>
-      </c>
-      <c r="AM161" t="s">
-        <v>2042</v>
-      </c>
-      <c r="AO161">
-        <v>1</v>
-      </c>
-      <c r="AP161" t="s">
+      <c r="AB161" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC161" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD161" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE161" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF161" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG161" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH161" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI161" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AJ161" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AK161" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AL161" s="3" t="s">
+        <v>2041</v>
+      </c>
+      <c r="AM161" s="3" t="s">
+        <v>2042</v>
+      </c>
+      <c r="AO161" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP161" s="3" t="s">
         <v>2057</v>
       </c>
     </row>

</xml_diff>